<commit_message>
SBERDOMA-1030 - refactor with global mappers
</commit_message>
<xml_diff>
--- a/apps/condo/domains/ticket/templates/en/TicketAnalyticsExportTemplate[status_property].xlsx
+++ b/apps/condo/domains/ticket/templates/en/TicketAnalyticsExportTemplate[status_property].xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Processing</t>
   </si>
   <si>
-    <t xml:space="preserve">Complete</t>
+    <t xml:space="preserve">Completed</t>
   </si>
   <si>
     <t xml:space="preserve">Canceled</t>
@@ -291,16 +291,16 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.36"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.77"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="11.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.69"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="1" width="11.63"/>
@@ -329,7 +329,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
@@ -352,7 +352,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="36.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="25.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>14</v>
       </c>

</xml_diff>